<commit_message>
now using Probennummer, fixed idx numbering and corrected test file
</commit_message>
<xml_diff>
--- a/files/full_list/fixed_list.xlsx
+++ b/files/full_list/fixed_list.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27018"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\varis_info\files\full_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50709FF5-4DAD-422F-8451-5A910C537603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="1725" windowWidth="21600" windowHeight="11385" activeTab="0"/>
+    <workbookView xWindow="6465" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -47,18 +36,12 @@
     <t>fgdg</t>
   </si>
   <si>
-    <t>dfgdfg</t>
-  </si>
-  <si>
     <t>6259-2-1</t>
   </si>
   <si>
     <t>w</t>
   </si>
   <si>
-    <t>gfhfgh</t>
-  </si>
-  <si>
     <t>fghfgh</t>
   </si>
   <si>
@@ -71,41 +54,59 @@
     <t>asdasd</t>
   </si>
   <si>
+    <t>6067-1-p</t>
+  </si>
+  <si>
+    <t>sdfgsdg</t>
+  </si>
+  <si>
+    <t>Vater</t>
+  </si>
+  <si>
+    <t>6067-1-m</t>
+  </si>
+  <si>
+    <t>fsdgsf</t>
+  </si>
+  <si>
+    <t>sg</t>
+  </si>
+  <si>
+    <t>Mutter</t>
+  </si>
+  <si>
+    <t>asda</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
     <t>m</t>
   </si>
   <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>6067-1-p</t>
-  </si>
-  <si>
-    <t>sdfgsdg</t>
-  </si>
-  <si>
-    <t>Vater</t>
-  </si>
-  <si>
-    <t>6067-1-m</t>
-  </si>
-  <si>
-    <t>fsdgsf</t>
-  </si>
-  <si>
-    <t>sg</t>
-  </si>
-  <si>
-    <t>Mutter</t>
-  </si>
-  <si>
-    <t>asda</t>
+    <t>Bdfgdfg</t>
+  </si>
+  <si>
+    <t>Edfgdfg</t>
+  </si>
+  <si>
+    <t>Fdfgdfg</t>
+  </si>
+  <si>
+    <t>Gdfgdfg</t>
+  </si>
+  <si>
+    <t>Hdfgdfg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,9 +115,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -137,112 +138,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -255,7 +173,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -550,16 +468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2250C52-0104-40E3-998D-F32F222F3722}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2250C52-0104-40E3-998D-F32F222F3722}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.424285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -594,213 +512,223 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15">
-      <c r="A3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" ht="15">
-      <c r="C4" s="1" t="s">
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>6969</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" ht="15">
-      <c r="C5" s="1" t="s">
+      <c r="I6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
-        <v>9696</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="15">
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="15">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:3" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:3" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="3:3" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:3" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="3:3" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="3:3" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="3:3" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" ht="15">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" ht="15">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" ht="15">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" ht="15">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" ht="15">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" ht="15">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" ht="15">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" ht="15">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" ht="15">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3" ht="15">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3" ht="15">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3" ht="15">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:3" ht="15">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:3" ht="15">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:3" ht="15">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:3" ht="15">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" ht="15">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="3:3" ht="15">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3" ht="15">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3" ht="15">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3" ht="15">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3" ht="15">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>